<commit_message>
removed conflicting label keys
</commit_message>
<xml_diff>
--- a/scripts f keys taken.xlsx
+++ b/scripts f keys taken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\ahk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D6362F-24A4-4B6F-B376-9F38AF5AC9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1E21CB-B59C-4B66-9F33-B743A2DAE02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{988935E9-0B57-47DD-B8E6-A709369EFA7D}"/>
   </bookViews>
@@ -324,7 +324,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
@@ -658,7 +659,7 @@
   <dimension ref="C2:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,345 +673,505 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="1"/>
+      <c r="G3" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>37</v>
       </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="G8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="I9" s="1" t="s">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="3:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="2"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="E15" s="1"/>
+      <c r="F15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="1" t="s">
+      <c r="G15" s="3"/>
+      <c r="H15" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="2"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="I19" s="1" t="s">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="I21" s="1" t="s">
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="2"/>
-      <c r="I22" s="1" t="s">
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="I23" s="1" t="s">
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="2"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G25" s="2"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G26" s="2"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="6">
         <v>1</v>
       </c>
-      <c r="G28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D29" s="5">
+      <c r="C29" s="1"/>
+      <c r="D29" s="6">
         <v>2</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="7" t="s">
         <v>61</v>
       </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D30" s="5">
+      <c r="C30" s="1"/>
+      <c r="D30" s="6">
         <v>3</v>
       </c>
-      <c r="G30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D31" s="5">
+      <c r="C31" s="1"/>
+      <c r="D31" s="6">
         <v>4</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D32" s="5">
+      <c r="C32" s="1"/>
+      <c r="D32" s="6">
         <v>5</v>
       </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
     </row>
     <row r="33" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D33" s="5">
+      <c r="D33" s="6">
         <v>6</v>
       </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D34" s="5">
+      <c r="D34" s="6">
         <v>7</v>
       </c>
-      <c r="G34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D35" s="5">
+      <c r="D35" s="6">
         <v>8</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="7" t="s">
         <v>63</v>
       </c>
+      <c r="H35" s="1"/>
     </row>
     <row r="36" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D36" s="5">
+      <c r="D36" s="6">
         <v>9</v>
       </c>
-      <c r="G36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="1"/>
     </row>
     <row r="43" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
+      <c r="D43" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="F43" s="1"/>
+      <c r="G43" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H43" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="44" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E44" s="1" t="s">
+      <c r="D44" s="1"/>
+      <c r="E44" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="F44" s="1"/>
+      <c r="G44" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H44" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="45" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G45" s="1" t="s">
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H45" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="46" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G46" s="1" t="s">
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="H46" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="47" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G47" s="1" t="s">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="H47" s="1"/>
     </row>
     <row r="48" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G48" s="1" t="s">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="H48" s="1"/>
     </row>
     <row r="49" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G49" s="1" t="s">
+      <c r="G49" s="2" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Open Excel elevated, updated excel doc
</commit_message>
<xml_diff>
--- a/scripts f keys taken.xlsx
+++ b/scripts f keys taken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\ahk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759FE0A1-AD9A-457E-B443-A0CDF476DF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1F309F-7B47-492D-9361-9BE22F063667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{988935E9-0B57-47DD-B8E6-A709369EFA7D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>f1</t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>ctrl+space -&gt; toggle active window always on top</t>
+  </si>
+  <si>
+    <t>Num/ -&gt; open excel elevated.</t>
+  </si>
+  <si>
+    <t>alt+r -&gt; reload script</t>
   </si>
 </sst>
 </file>
@@ -674,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6D84AE-EF5D-416A-8D76-EC512DB5CC0A}">
   <dimension ref="C2:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,7 +1180,9 @@
     </row>
     <row r="47" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
+      <c r="E47" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="F47" s="1"/>
       <c r="G47" s="2" t="s">
         <v>66</v>
@@ -1183,7 +1191,9 @@
     </row>
     <row r="48" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
+      <c r="E48" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="F48" s="1"/>
       <c r="G48" s="8" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
comments, mark out redundant audition hotkey
</commit_message>
<xml_diff>
--- a/scripts f keys taken.xlsx
+++ b/scripts f keys taken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\ahk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0199C89-A1C4-4A41-A6D0-4F8CA0F26C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB94350-44F5-44CD-BB37-8E64A567277B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{988935E9-0B57-47DD-B8E6-A709369EFA7D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t>f1</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>botshi</t>
-  </si>
-  <si>
-    <t>limiter</t>
   </si>
   <si>
     <t>mouse</t>
@@ -690,7 +687,7 @@
   <dimension ref="C2:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,7 +702,7 @@
   <sheetData>
     <row r="2" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
@@ -718,10 +715,10 @@
         <v>26</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
@@ -730,11 +727,11 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -745,11 +742,11 @@
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -760,11 +757,11 @@
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -777,7 +774,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="1"/>
       <c r="G6" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -788,11 +785,11 @@
         <v>4</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -807,7 +804,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
@@ -820,7 +817,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="1"/>
       <c r="I9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
@@ -829,7 +826,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -855,7 +852,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="3"/>
@@ -870,7 +867,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -892,12 +889,10 @@
         <v>12</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="F15" s="1"/>
       <c r="G15" s="3"/>
       <c r="H15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I15" s="1"/>
     </row>
@@ -909,10 +904,10 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -952,7 +947,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="1"/>
       <c r="I19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
@@ -976,7 +971,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="1"/>
       <c r="I21" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
@@ -989,7 +984,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="1"/>
       <c r="I22" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
@@ -1002,7 +997,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="1"/>
       <c r="I23" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
@@ -1011,7 +1006,7 @@
         <v>21</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="3"/>
@@ -1026,7 +1021,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1039,14 +1034,14 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D28" s="6">
         <v>1</v>
@@ -1065,7 +1060,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -1089,7 +1084,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -1130,7 +1125,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H35" s="1"/>
     </row>
@@ -1145,85 +1140,85 @@
     </row>
     <row r="37" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
+        <v>77</v>
+      </c>
+      <c r="G37" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="43" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D44" s="1"/>
       <c r="E44" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D45" s="1"/>
       <c r="E45" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D46" s="1"/>
       <c r="E46" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D47" s="1"/>
       <c r="E47" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D48" s="1"/>
       <c r="E48" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H48" s="1"/>
     </row>

</xml_diff>

<commit_message>
Script to close all stream applications
added new excel file as well
</commit_message>
<xml_diff>
--- a/scripts f keys taken.xlsx
+++ b/scripts f keys taken.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\ahk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB94350-44F5-44CD-BB37-8E64A567277B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E25869C-2754-4AE1-AB0C-CCAE47447E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{988935E9-0B57-47DD-B8E6-A709369EFA7D}"/>
+    <workbookView xWindow="8775" yWindow="1665" windowWidth="28800" windowHeight="15435" xr2:uid="{988935E9-0B57-47DD-B8E6-A709369EFA7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
   <si>
     <t>f1</t>
   </si>
@@ -271,6 +271,15 @@
   </si>
   <si>
     <t>Launch excel elevated</t>
+  </si>
+  <si>
+    <t>Close all stream windows</t>
+  </si>
+  <si>
+    <t>open stream queue</t>
+  </si>
+  <si>
+    <t>random mii wii hotkey</t>
   </si>
 </sst>
 </file>
@@ -686,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6D84AE-EF5D-416A-8D76-EC512DB5CC0A}">
   <dimension ref="C2:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,7 +897,9 @@
       <c r="D15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="3"/>
       <c r="H15" s="2" t="s">
@@ -942,7 +953,9 @@
       <c r="D19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="3"/>
       <c r="H19" s="1"/>
@@ -955,7 +968,6 @@
       <c r="D20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="3"/>
       <c r="H20" s="1"/>
@@ -966,7 +978,9 @@
       <c r="D21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="3"/>
       <c r="H21" s="1"/>

</xml_diff>

<commit_message>
streamdeck launch individual scripts moved some functionality from the main script into individual scripts to allow the opening up of those hotkeys
</commit_message>
<xml_diff>
--- a/scripts f keys taken.xlsx
+++ b/scripts f keys taken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\ahk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E4474B-4CF7-47AC-9033-2B87550F7376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91AAAC0-6D89-419A-9CF9-049E37FD749F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8775" yWindow="1665" windowWidth="28800" windowHeight="15435" xr2:uid="{988935E9-0B57-47DD-B8E6-A709369EFA7D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="84">
   <si>
     <t>f1</t>
   </si>
@@ -205,15 +205,6 @@
   </si>
   <si>
     <t>scale effects</t>
-  </si>
-  <si>
-    <t>ctrl+1&gt;3 -&gt; scale presets</t>
-  </si>
-  <si>
-    <t>ctrl+shift+1&gt;3 -&gt; speed macros</t>
-  </si>
-  <si>
-    <t>ctrl+4&gt;6 -&gt; speed macros</t>
   </si>
   <si>
     <t>github</t>
@@ -711,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6D84AE-EF5D-416A-8D76-EC512DB5CC0A}">
   <dimension ref="C2:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,7 +747,7 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -771,7 +762,7 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -785,7 +776,7 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -798,7 +789,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="1"/>
       <c r="G6" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -813,7 +804,7 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -834,7 +825,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="3"/>
@@ -846,7 +837,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -872,7 +863,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="3"/>
@@ -907,7 +898,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="3"/>
@@ -960,7 +951,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="3"/>
@@ -984,7 +975,7 @@
         <v>18</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="3"/>
@@ -1047,7 +1038,7 @@
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>0</v>
@@ -1161,7 +1152,7 @@
       </c>
       <c r="G50" s="1"/>
       <c r="I50" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
@@ -1170,7 +1161,7 @@
       </c>
       <c r="G51" s="3"/>
       <c r="I51" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
@@ -1179,7 +1170,7 @@
       </c>
       <c r="G52" s="3"/>
       <c r="I52" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="3:9" x14ac:dyDescent="0.25">
@@ -1283,15 +1274,15 @@
     </row>
     <row r="64" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>39</v>
@@ -1299,7 +1290,7 @@
     </row>
     <row r="66" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>39</v>
@@ -1336,11 +1327,11 @@
     <row r="72" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D72" s="1"/>
       <c r="E72" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F72" s="1"/>
-      <c r="G72" s="2" t="s">
-        <v>57</v>
+      <c r="G72" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>46</v>
@@ -1349,11 +1340,11 @@
     <row r="73" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D73" s="1"/>
       <c r="E73" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F73" s="1"/>
-      <c r="G73" s="2" t="s">
-        <v>58</v>
+      <c r="G73" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>51</v>
@@ -1362,36 +1353,27 @@
     <row r="74" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D74" s="1"/>
       <c r="E74" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F74" s="1"/>
-      <c r="G74" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="H74" s="1"/>
     </row>
     <row r="75" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D75" s="1"/>
       <c r="E75" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F75" s="1"/>
-      <c r="G75" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="H75" s="1"/>
     </row>
     <row r="76" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E76" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G76" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E77" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preparing for second keyboard
</commit_message>
<xml_diff>
--- a/scripts f keys taken.xlsx
+++ b/scripts f keys taken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\ahk\ahk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A444B8-3B4D-4FC0-8ADE-65A6C67E8AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8966A4E5-5641-4C21-A0E0-7BFC8E0CCEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{988935E9-0B57-47DD-B8E6-A709369EFA7D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="95">
   <si>
     <t>f1</t>
   </si>
@@ -311,6 +311,15 @@
   </si>
   <si>
     <t>Open highlighted text in ahk documentation</t>
+  </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t>Second Keyboard</t>
+  </si>
+  <si>
+    <t>backspace</t>
   </si>
 </sst>
 </file>
@@ -724,14 +733,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6D84AE-EF5D-416A-8D76-EC512DB5CC0A}">
-  <dimension ref="C2:I85"/>
+  <dimension ref="C2:I142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
@@ -766,13 +776,7 @@
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="8" t="s">
-        <v>60</v>
-      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
@@ -781,13 +785,7 @@
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="8" t="s">
-        <v>62</v>
-      </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -795,13 +793,7 @@
       <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
@@ -812,9 +804,6 @@
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
@@ -827,9 +816,6 @@
         <v>32</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="8" t="s">
-        <v>64</v>
-      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
@@ -1158,6 +1144,9 @@
         <v>20</v>
       </c>
       <c r="G49" s="1"/>
+      <c r="I49" s="8" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D50" s="1" t="s">
@@ -1395,7 +1384,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D81" s="1"/>
       <c r="E81" s="8" t="s">
         <v>58</v>
@@ -1406,7 +1395,7 @@
       </c>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D82" s="1"/>
       <c r="E82" s="8" t="s">
         <v>59</v>
@@ -1417,7 +1406,7 @@
       </c>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E83" s="8" t="s">
         <v>77</v>
       </c>
@@ -1425,7 +1414,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E84" s="8" t="s">
         <v>82</v>
       </c>
@@ -1433,10 +1422,289 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E85" s="8" t="s">
         <v>78</v>
       </c>
+    </row>
+    <row r="89" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>93</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E89" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D90" s="1"/>
+      <c r="E90" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D91" s="1"/>
+      <c r="E91" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D92" s="1"/>
+      <c r="E92" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D93" s="1"/>
+      <c r="E93" s="6">
+        <v>5</v>
+      </c>
+      <c r="G93" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="94" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D94" s="1"/>
+      <c r="E94" s="6">
+        <v>6</v>
+      </c>
+      <c r="G94" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="95" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D95" s="1"/>
+      <c r="E95" s="6">
+        <v>7</v>
+      </c>
+      <c r="G95" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="96" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D96" s="1"/>
+      <c r="E96" s="6">
+        <v>8</v>
+      </c>
+      <c r="G96" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="97" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D97" s="1"/>
+      <c r="E97" s="6">
+        <v>9</v>
+      </c>
+      <c r="G97" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="98" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D98" s="1"/>
+      <c r="E98" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="99" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D99" s="1"/>
+      <c r="E99" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="100" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D100" s="1"/>
+      <c r="E100" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="101" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D101" s="1"/>
+      <c r="E101" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="102" spans="4:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E102" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="103" spans="4:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+    </row>
+    <row r="105" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D105" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="106" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D106" s="1"/>
+      <c r="E106" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="107" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D107" s="1"/>
+      <c r="E107" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="108" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+    </row>
+    <row r="109" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+    </row>
+    <row r="110" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+    </row>
+    <row r="111" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+    </row>
+    <row r="112" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D112" s="1"/>
+      <c r="E112" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="113" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+    </row>
+    <row r="114" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+    </row>
+    <row r="115" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+    </row>
+    <row r="116" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+    </row>
+    <row r="117" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+    </row>
+    <row r="118" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D118" s="1"/>
+      <c r="E118" s="1"/>
+    </row>
+    <row r="119" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+    </row>
+    <row r="120" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D120" s="1"/>
+      <c r="E120" s="1"/>
+    </row>
+    <row r="121" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D121" s="1"/>
+      <c r="E121" s="1"/>
+    </row>
+    <row r="122" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D122" s="1"/>
+      <c r="E122" s="1"/>
+    </row>
+    <row r="123" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D123" s="1"/>
+      <c r="E123" s="1"/>
+    </row>
+    <row r="124" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D124" s="1"/>
+      <c r="E124" s="1"/>
+    </row>
+    <row r="125" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D125" s="1"/>
+      <c r="E125" s="1"/>
+    </row>
+    <row r="126" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
+    </row>
+    <row r="127" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D127" s="1"/>
+      <c r="E127" s="1"/>
+    </row>
+    <row r="128" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D128" s="1"/>
+      <c r="E128" s="1"/>
+    </row>
+    <row r="129" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D129" s="1"/>
+      <c r="E129" s="1"/>
+    </row>
+    <row r="130" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D130" s="1"/>
+      <c r="E130" s="1"/>
+    </row>
+    <row r="131" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D131" s="1"/>
+      <c r="E131" s="1"/>
+    </row>
+    <row r="132" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
+    </row>
+    <row r="133" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D133" s="1"/>
+      <c r="E133" s="1"/>
+    </row>
+    <row r="134" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D134" s="1"/>
+      <c r="E134" s="1"/>
+    </row>
+    <row r="135" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D135" s="1"/>
+      <c r="E135" s="1"/>
+    </row>
+    <row r="136" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D136" s="1"/>
+      <c r="E136" s="1"/>
+    </row>
+    <row r="137" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D137" s="1"/>
+      <c r="E137" s="1"/>
+    </row>
+    <row r="138" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D138" s="1"/>
+      <c r="E138" s="1"/>
+    </row>
+    <row r="139" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D139" s="1"/>
+      <c r="E139" s="1"/>
+    </row>
+    <row r="140" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D140" s="1"/>
+      <c r="E140" s="1"/>
+    </row>
+    <row r="141" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D141" s="1"/>
+      <c r="E141" s="1"/>
+    </row>
+    <row r="142" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D142" s="1"/>
+      <c r="E142" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Middle mouse premiere changes
</commit_message>
<xml_diff>
--- a/scripts f keys taken.xlsx
+++ b/scripts f keys taken.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\ahk\ahk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6069C2-C08A-45E2-A161-B5327A573E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE862C9-2A95-406B-8A78-4BA801C77555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{988935E9-0B57-47DD-B8E6-A709369EFA7D}"/>
+    <workbookView xWindow="8910" yWindow="4845" windowWidth="28800" windowHeight="15435" xr2:uid="{988935E9-0B57-47DD-B8E6-A709369EFA7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -735,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6D84AE-EF5D-416A-8D76-EC512DB5CC0A}">
   <dimension ref="C2:I142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G80" sqref="G80"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,9 +996,6 @@
       <c r="F23" s="1"/>
       <c r="G23" s="3"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="2" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
@@ -1058,85 +1055,91 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D33" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D34" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D35" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D36" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D37" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D38" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D40" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D41" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D42" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D43" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D44" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D45" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D46" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D47" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="48" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="I47" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D48" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
@@ -1171,9 +1174,6 @@
         <v>23</v>
       </c>
       <c r="G52" s="3"/>
-      <c r="I52" s="2" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="55" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C55" s="1" t="s">

</xml_diff>

<commit_message>
psProp() - Photoshop to MS_Functions also cleaned up the QMK Keyboard file
</commit_message>
<xml_diff>
--- a/scripts f keys taken.xlsx
+++ b/scripts f keys taken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\ahk\ahk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0ACE00-80A9-4086-B058-FC52E7CFDC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F1839E-4180-4A04-8522-BF5B4BD9A410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8910" yWindow="4845" windowWidth="28800" windowHeight="15435" xr2:uid="{988935E9-0B57-47DD-B8E6-A709369EFA7D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="109">
   <si>
     <t>f1</t>
   </si>
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>ctrl+space -&gt; toggle active window always on top</t>
-  </si>
-  <si>
-    <t>Num/ -&gt; open excel elevated.</t>
   </si>
   <si>
     <t>alt+r -&gt; reload script</t>
@@ -323,6 +320,48 @@
   </si>
   <si>
     <t>all mii wii song</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>enter</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>pgUp</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>down</t>
+  </si>
+  <si>
+    <t>pgdown</t>
+  </si>
+  <si>
+    <t>ins</t>
+  </si>
+  <si>
+    <t>del</t>
+  </si>
+  <si>
+    <t>Numlock -&gt; open excel elevated.</t>
   </si>
 </sst>
 </file>
@@ -738,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6D84AE-EF5D-416A-8D76-EC512DB5CC0A}">
   <dimension ref="C2:I142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,6 +866,7 @@
       <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="E8" s="5"/>
       <c r="F8" s="1"/>
       <c r="G8" s="3"/>
       <c r="H8" s="1"/>
@@ -872,7 +912,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="3"/>
@@ -941,7 +981,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="3"/>
@@ -954,7 +994,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="3"/>
@@ -1036,13 +1076,13 @@
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
@@ -1144,7 +1184,7 @@
         <v>19</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
@@ -1153,7 +1193,7 @@
       </c>
       <c r="G49" s="1"/>
       <c r="I49" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
@@ -1162,7 +1202,7 @@
       </c>
       <c r="G50" s="1"/>
       <c r="I50" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
@@ -1171,7 +1211,7 @@
       </c>
       <c r="G51" s="3"/>
       <c r="I51" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
@@ -1276,12 +1316,12 @@
     </row>
     <row r="64" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>37</v>
@@ -1289,7 +1329,7 @@
     </row>
     <row r="66" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>37</v>
@@ -1297,37 +1337,37 @@
     </row>
     <row r="67" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
+        <v>85</v>
+      </c>
+      <c r="D70" t="s">
         <v>86</v>
       </c>
-      <c r="D70" t="s">
-        <v>87</v>
-      </c>
       <c r="E70" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="77" spans="3:9" x14ac:dyDescent="0.25">
@@ -1378,7 +1418,7 @@
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>48</v>
@@ -1387,102 +1427,99 @@
     <row r="81" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D81" s="1"/>
       <c r="E81" s="8" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H81" s="1"/>
     </row>
     <row r="82" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D82" s="1"/>
       <c r="E82" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H82" s="1"/>
     </row>
     <row r="83" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E83" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E84" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G84" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="G84" s="8" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="85" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E85" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="89" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>50</v>
       </c>
       <c r="E89" s="6">
-        <v>1</v>
-      </c>
-      <c r="G89" s="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="90" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D90" s="1"/>
       <c r="E90" s="6">
-        <v>2</v>
-      </c>
-      <c r="G90" s="7" t="s">
-        <v>51</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G90" s="2"/>
     </row>
     <row r="91" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D91" s="1"/>
       <c r="E91" s="6">
-        <v>3</v>
-      </c>
-      <c r="G91" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="92" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D92" s="1"/>
       <c r="E92" s="6">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G92" s="2"/>
     </row>
     <row r="93" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D93" s="1"/>
       <c r="E93" s="6">
-        <v>5</v>
-      </c>
-      <c r="G93" s="8" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D94" s="1"/>
       <c r="E94" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G94" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="95" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D95" s="1"/>
       <c r="E95" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G95" s="8" t="s">
         <v>60</v>
@@ -1491,125 +1528,150 @@
     <row r="96" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D96" s="1"/>
       <c r="E96" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G96" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="97" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D97" s="1"/>
       <c r="E97" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="98" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D98" s="1"/>
-      <c r="E98" s="1" t="s">
-        <v>65</v>
+      <c r="E98" s="6">
+        <v>9</v>
+      </c>
+      <c r="G98" s="8" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="99" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D99" s="1"/>
       <c r="E99" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
     </row>
     <row r="100" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D100" s="1"/>
-      <c r="E100" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>30</v>
+      <c r="E100" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="101" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D101" s="1"/>
       <c r="E101" s="1" t="s">
-        <v>85</v>
+        <v>71</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="102" spans="4:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E102" s="1" t="s">
-        <v>94</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F102"/>
       <c r="G102" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="103" spans="4:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="103" spans="4:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E103" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
     <row r="104" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
+      <c r="E104" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="105" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D105" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="D105" s="1"/>
       <c r="E105" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
+      </c>
+      <c r="F105" s="1"/>
+      <c r="G105" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="106" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D106" s="1"/>
       <c r="E106" s="1" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="107" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D107" s="1"/>
-      <c r="E107" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="E107" s="1"/>
     </row>
     <row r="108" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D108" s="1"/>
-      <c r="E108" s="1"/>
+      <c r="E108" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="109" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D109" s="1"/>
-      <c r="E109" s="1"/>
+      <c r="E109" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="110" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
+      <c r="E110" s="1" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="111" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D111" s="1"/>
-      <c r="E111" s="1"/>
+      <c r="E111" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="112" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D112" s="1"/>
       <c r="E112" s="1" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
     </row>
     <row r="113" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D113" s="1"/>
-      <c r="E113" s="1"/>
+      <c r="E113" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="114" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D114" s="1"/>
-      <c r="E114" s="1"/>
+      <c r="E114" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="115" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
+      <c r="E115" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="116" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D116" s="1"/>
-      <c r="E116" s="1"/>
+      <c r="E116" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="117" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D117" s="1"/>
-      <c r="E117" s="1"/>
+      <c r="E117" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="118" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D118" s="1"/>

</xml_diff>

<commit_message>
Fkey auto launch -> MS_Functions
</commit_message>
<xml_diff>
--- a/scripts f keys taken.xlsx
+++ b/scripts f keys taken.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\ahk\ahk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F1839E-4180-4A04-8522-BF5B4BD9A410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C6217F-35E2-45AE-8B7C-FAE4755C2C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8910" yWindow="4845" windowWidth="28800" windowHeight="15435" xr2:uid="{988935E9-0B57-47DD-B8E6-A709369EFA7D}"/>
+    <workbookView xWindow="38280" yWindow="2700" windowWidth="29040" windowHeight="15840" xr2:uid="{988935E9-0B57-47DD-B8E6-A709369EFA7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="111">
   <si>
     <t>f1</t>
   </si>
@@ -129,9 +129,6 @@
     <t>premiere</t>
   </si>
   <si>
-    <t>firefox</t>
-  </si>
-  <si>
     <t>putting things here requires being careful</t>
   </si>
   <si>
@@ -174,12 +171,6 @@
     <t>ctrl+p -&gt; save replay</t>
   </si>
   <si>
-    <t>alt+g -&gt; drag drop preset</t>
-  </si>
-  <si>
-    <t>alt+p -&gt; drag drop preset</t>
-  </si>
-  <si>
     <t>ctrl+shift+r -&gt; run ahk script to record replays in obs (ifwinEXIST, obs)</t>
   </si>
   <si>
@@ -204,9 +195,6 @@
     <t>alt+h -&gt; horizontal flip preset</t>
   </si>
   <si>
-    <t>alt+a -&gt; edit main script</t>
-  </si>
-  <si>
     <t>ctrl+space -&gt; toggle active window always on top</t>
   </si>
   <si>
@@ -229,9 +217,6 @@
   </si>
   <si>
     <t>/</t>
-  </si>
-  <si>
-    <t>Launch excel elevated</t>
   </si>
   <si>
     <t>random mii wii hotkey</t>
@@ -362,6 +347,27 @@
   </si>
   <si>
     <t>Numlock -&gt; open excel elevated.</t>
+  </si>
+  <si>
+    <t>alt+g -&gt; blur preset</t>
+  </si>
+  <si>
+    <t>alt+p -&gt; parametric eq preset</t>
+  </si>
+  <si>
+    <t>pgup</t>
+  </si>
+  <si>
+    <t>pausebreak</t>
+  </si>
+  <si>
+    <t>Launch excel</t>
+  </si>
+  <si>
+    <t>launch window spy</t>
+  </si>
+  <si>
+    <t>launch firefox</t>
   </si>
 </sst>
 </file>
@@ -775,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6D84AE-EF5D-416A-8D76-EC512DB5CC0A}">
-  <dimension ref="C2:I142"/>
+  <dimension ref="B2:I142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,7 +800,7 @@
   <sheetData>
     <row r="2" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
@@ -807,10 +813,10 @@
         <v>26</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
@@ -855,7 +861,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="1"/>
       <c r="H7" s="1"/>
@@ -886,7 +892,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -912,7 +918,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="3"/>
@@ -960,7 +966,7 @@
         <v>28</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -981,7 +987,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="3"/>
@@ -994,7 +1000,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="3"/>
@@ -1008,7 +1014,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="3"/>
       <c r="H20" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I20" s="1"/>
     </row>
@@ -1048,7 +1054,7 @@
         <v>21</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="3"/>
@@ -1076,13 +1082,13 @@
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
@@ -1176,7 +1182,7 @@
         <v>18</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.25">
@@ -1184,7 +1190,7 @@
         <v>19</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
@@ -1193,7 +1199,7 @@
       </c>
       <c r="G49" s="1"/>
       <c r="I49" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
@@ -1202,7 +1208,7 @@
       </c>
       <c r="G50" s="1"/>
       <c r="I50" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
@@ -1211,7 +1217,7 @@
       </c>
       <c r="G51" s="3"/>
       <c r="I51" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
@@ -1222,7 +1228,7 @@
     </row>
     <row r="55" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C55" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D55" s="6">
         <v>1</v>
@@ -1260,7 +1266,7 @@
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -1301,7 +1307,7 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H62" s="1"/>
     </row>
@@ -1316,361 +1322,364 @@
     </row>
     <row r="64" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="67" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
-        <v>84</v>
-      </c>
-      <c r="G67" s="8" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D70" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>90</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="73" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>106</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="74" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>100</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="75" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>107</v>
+      </c>
+      <c r="E75" s="8" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D77" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="2" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D78" s="1"/>
       <c r="E78" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="2" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="79" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D79" s="1"/>
       <c r="E79" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="80" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D80" s="1"/>
       <c r="E80" s="8" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="81" spans="3:8" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D81" s="1"/>
       <c r="E81" s="8" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D82" s="1"/>
       <c r="E82" s="8" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E83" s="8" t="s">
         <v>76</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="84" spans="3:8" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E84" s="8" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="85" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E85" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="89" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C89" t="s">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>87</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D89" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C90" s="1"/>
+      <c r="D90" s="6">
+        <v>1</v>
+      </c>
+      <c r="G90" s="2"/>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C91" s="1"/>
+      <c r="D91" s="6">
+        <v>2</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C92" s="1"/>
+      <c r="D92" s="6">
+        <v>3</v>
+      </c>
+      <c r="G92" s="2"/>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C93" s="1"/>
+      <c r="D93" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C94" s="1"/>
+      <c r="D94" s="6">
+        <v>5</v>
+      </c>
+      <c r="G94" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C95" s="1"/>
+      <c r="D95" s="6">
+        <v>6</v>
+      </c>
+      <c r="G95" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C96" s="1"/>
+      <c r="D96" s="6">
+        <v>7</v>
+      </c>
+      <c r="G96" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="97" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C97" s="1"/>
+      <c r="D97" s="6">
+        <v>8</v>
+      </c>
+      <c r="G97" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="98" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C98" s="1"/>
+      <c r="D98" s="6">
+        <v>9</v>
+      </c>
+      <c r="G98" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="99" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C99" s="1"/>
+      <c r="D99" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C100" s="1"/>
+      <c r="D100" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="101" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C101" s="1"/>
+      <c r="D101" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="102" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D102" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F102"/>
+    </row>
+    <row r="103" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D103" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D89" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E89" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D90" s="1"/>
-      <c r="E90" s="6">
-        <v>1</v>
-      </c>
-      <c r="G90" s="2"/>
-    </row>
-    <row r="91" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D91" s="1"/>
-      <c r="E91" s="6">
-        <v>2</v>
-      </c>
-      <c r="G91" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="92" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D92" s="1"/>
-      <c r="E92" s="6">
-        <v>3</v>
-      </c>
-      <c r="G92" s="2"/>
-    </row>
-    <row r="93" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D93" s="1"/>
-      <c r="E93" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="94" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D94" s="1"/>
-      <c r="E94" s="6">
-        <v>5</v>
-      </c>
-      <c r="G94" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="95" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D95" s="1"/>
-      <c r="E95" s="6">
-        <v>6</v>
-      </c>
-      <c r="G95" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="96" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D96" s="1"/>
-      <c r="E96" s="6">
-        <v>7</v>
-      </c>
-      <c r="G96" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="97" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D97" s="1"/>
-      <c r="E97" s="6">
-        <v>8</v>
-      </c>
-      <c r="G97" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="98" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D98" s="1"/>
-      <c r="E98" s="6">
-        <v>9</v>
-      </c>
-      <c r="G98" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="99" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D99" s="1"/>
-      <c r="E99" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="100" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D100" s="1"/>
-      <c r="E100" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="101" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D101" s="1"/>
-      <c r="E101" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="102" spans="4:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E102" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F102"/>
-      <c r="G102" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="103" spans="4:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E103" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="104" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D104" s="1"/>
-      <c r="E104" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="105" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D105" s="1"/>
-      <c r="E105" s="1" t="s">
-        <v>93</v>
+    </row>
+    <row r="104" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C104" s="1"/>
+      <c r="D104" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="105" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C105" s="1"/>
+      <c r="D105" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="F105" s="1"/>
-      <c r="G105" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="106" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D106" s="1"/>
-      <c r="E106" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="107" spans="4:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C106" s="1"/>
+      <c r="D106" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="107" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
     </row>
-    <row r="108" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D108" s="1"/>
-      <c r="E108" s="1" t="s">
+    <row r="108" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D108" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="109" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D109" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="110" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D110" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="111" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D111" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="112" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D112" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="113" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D113" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="109" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D109" s="1"/>
-      <c r="E109" s="1" t="s">
+    <row r="114" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D114" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="110" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D110" s="1"/>
-      <c r="E110" s="1" t="s">
+    <row r="115" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D115" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="111" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D111" s="1"/>
-      <c r="E111" s="1" t="s">
+    <row r="116" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D116" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="112" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D112" s="1"/>
-      <c r="E112" s="1" t="s">
+    <row r="117" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D117" s="1" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="113" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D113" s="1"/>
-      <c r="E113" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="114" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D114" s="1"/>
-      <c r="E114" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="115" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D115" s="1"/>
-      <c r="E115" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="116" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D116" s="1"/>
-      <c r="E116" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="117" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D117" s="1"/>
-      <c r="E117" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="118" spans="4:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pre Release 1 - preparation
</commit_message>
<xml_diff>
--- a/scripts f keys taken.xlsx
+++ b/scripts f keys taken.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\ahk\ahk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A027407-5732-4BD4-85FB-14ED2BAC569E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EF9CA3-BFFB-4ACC-AC19-3927285D48C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2700" windowWidth="29040" windowHeight="15840" xr2:uid="{988935E9-0B57-47DD-B8E6-A709369EFA7D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="105">
   <si>
     <t>f1</t>
   </si>
@@ -181,9 +181,6 @@
   </si>
   <si>
     <t>scale effects</t>
-  </si>
-  <si>
-    <t>github</t>
   </si>
   <si>
     <t>alt+h -&gt; horizontal flip preset</t>
@@ -265,9 +262,6 @@
     <t>ctrl + middle mouse click</t>
   </si>
   <si>
-    <t>manual scale input</t>
-  </si>
-  <si>
     <t>NumLock</t>
   </si>
   <si>
@@ -310,36 +304,9 @@
     <t>*</t>
   </si>
   <si>
-    <t>home</t>
-  </si>
-  <si>
-    <t>up</t>
-  </si>
-  <si>
-    <t>pgUp</t>
-  </si>
-  <si>
-    <t>left</t>
-  </si>
-  <si>
-    <t>right</t>
-  </si>
-  <si>
-    <t>end</t>
-  </si>
-  <si>
-    <t>down</t>
-  </si>
-  <si>
     <t>pgdown</t>
   </si>
   <si>
-    <t>ins</t>
-  </si>
-  <si>
-    <t>del</t>
-  </si>
-  <si>
     <t>Numlock -&gt; open excel elevated.</t>
   </si>
   <si>
@@ -364,13 +331,25 @@
     <t>launch firefox</t>
   </si>
   <si>
-    <t>open/switch to explorer. * + - opens new explorer</t>
-  </si>
-  <si>
     <t>open/switch to premiere</t>
   </si>
   <si>
     <t>Photoshop</t>
+  </si>
+  <si>
+    <t>scroll lock</t>
+  </si>
+  <si>
+    <t>Ralt + p -&gt; pull out the project window</t>
+  </si>
+  <si>
+    <t>open/switch to explorer. - + * opens new explorer</t>
+  </si>
+  <si>
+    <t>NumLock + 7</t>
+  </si>
+  <si>
+    <t>input manual scale</t>
   </si>
 </sst>
 </file>
@@ -784,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6D84AE-EF5D-416A-8D76-EC512DB5CC0A}">
-  <dimension ref="A2:J142"/>
+  <dimension ref="A2:J145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,7 +803,7 @@
         <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
@@ -899,9 +878,7 @@
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -912,9 +889,6 @@
       <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -926,7 +900,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="3"/>
@@ -995,7 +969,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="3"/>
@@ -1008,7 +982,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="3"/>
@@ -1090,14 +1064,12 @@
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G29" s="8" t="s">
-        <v>76</v>
-      </c>
+      <c r="G29" s="1"/>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D30" s="1" t="s">
@@ -1198,7 +1170,7 @@
         <v>19</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
@@ -1207,7 +1179,7 @@
       </c>
       <c r="G49" s="1"/>
       <c r="I49" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
@@ -1216,7 +1188,7 @@
       </c>
       <c r="G50" s="1"/>
       <c r="I50" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
@@ -1225,7 +1197,7 @@
       </c>
       <c r="G51" s="3"/>
       <c r="I51" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
@@ -1325,12 +1297,12 @@
     </row>
     <row r="64" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>34</v>
@@ -1338,7 +1310,7 @@
     </row>
     <row r="66" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>34</v>
@@ -1346,132 +1318,129 @@
     </row>
     <row r="67" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="70" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D70" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="71" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
+        <v>78</v>
+      </c>
+      <c r="E71" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="E71" s="8" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="72" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
+        <v>79</v>
+      </c>
+      <c r="E72" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="E72" s="8" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="73" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="75" spans="3:10" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="75" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="77" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D77" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="76" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>100</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D78" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="E78" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="F77" s="1"/>
-      <c r="G77" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J77" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D78" s="1"/>
-      <c r="E78" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="J78" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D79" s="1"/>
-      <c r="E79" s="8" t="s">
-        <v>51</v>
+      <c r="E79" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="F79" s="1"/>
-      <c r="G79" s="8" t="s">
-        <v>50</v>
+      <c r="G79" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="80" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D80" s="1"/>
       <c r="E80" s="8" t="s">
-        <v>101</v>
+        <v>50</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H80" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D81" s="1"/>
       <c r="E81" s="8" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H81" s="1"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D82" s="1"/>
       <c r="E82" s="8" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="8" t="s">
@@ -1479,244 +1448,237 @@
       </c>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D83" s="1"/>
       <c r="E83" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F83" s="1"/>
+      <c r="G83" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H83" s="1"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E84" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G84" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E85" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G85" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G83" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E84" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G84" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>85</v>
-      </c>
-      <c r="C89" s="1" t="s">
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G86" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>83</v>
+      </c>
+      <c r="C90" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D89" s="6">
+      <c r="D90" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C90" s="1"/>
-      <c r="D90" s="6">
-        <v>1</v>
-      </c>
-      <c r="G90" s="2"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C91" s="1"/>
       <c r="D91" s="6">
-        <v>2</v>
-      </c>
-      <c r="G91" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="G91" s="2"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C92" s="1"/>
       <c r="D92" s="6">
-        <v>3</v>
-      </c>
-      <c r="G92" s="2"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G92" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C93" s="1"/>
       <c r="D93" s="6">
-        <v>4</v>
-      </c>
-      <c r="G93" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G93" s="2"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C94" s="1"/>
       <c r="D94" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G94" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C95" s="1"/>
       <c r="D95" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G95" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C96" s="1"/>
       <c r="D96" s="6">
-        <v>7</v>
-      </c>
-      <c r="G96" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="J96" s="8" t="s">
-        <v>53</v>
+        <v>6</v>
+      </c>
+      <c r="G96" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="97" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C97" s="1"/>
       <c r="D97" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J97" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="98" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C98" s="1"/>
       <c r="D98" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G98" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J98" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="99" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C99" s="1"/>
-      <c r="D99" s="1" t="s">
-        <v>58</v>
+      <c r="D99" s="6">
+        <v>9</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="J99" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="100" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C100" s="1"/>
-      <c r="D100" t="s">
-        <v>88</v>
+      <c r="D100" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G100" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="101" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C101" s="1"/>
-      <c r="D101" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="102" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="102" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F102"/>
+        <v>102</v>
+      </c>
     </row>
     <row r="103" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D103" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G103" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="104" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C104" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F103"/>
+    </row>
+    <row r="104" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D104" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
+      </c>
+      <c r="G104" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="105" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F105" s="1"/>
-    </row>
-    <row r="106" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C106" s="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="106" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D106" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="107" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D107" s="1"/>
-      <c r="E107" s="1"/>
-    </row>
+        <v>103</v>
+      </c>
+      <c r="G106" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="107" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="108" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C108" s="1"/>
       <c r="D108" s="1" t="s">
-        <v>91</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="F108" s="1"/>
     </row>
     <row r="109" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="110" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D110" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
     </row>
     <row r="111" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D111" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="D111" s="1"/>
     </row>
     <row r="112" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D112" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="D112" s="1"/>
     </row>
     <row r="113" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D113" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="D113" s="1"/>
     </row>
     <row r="114" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D114" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="D114" s="1"/>
     </row>
     <row r="115" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D115" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="D115" s="1"/>
     </row>
     <row r="116" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D116" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="D116" s="1"/>
     </row>
     <row r="117" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D117" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="D117" s="1"/>
     </row>
     <row r="118" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D118" s="1"/>
-      <c r="E118" s="1"/>
     </row>
     <row r="119" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D119" s="1"/>
-      <c r="E119" s="1"/>
     </row>
     <row r="120" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D120" s="1"/>
-      <c r="E120" s="1"/>
     </row>
     <row r="121" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D121" s="1"/>
@@ -1805,6 +1767,18 @@
     <row r="142" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
+    </row>
+    <row r="143" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D143" s="1"/>
+      <c r="E143" s="1"/>
+    </row>
+    <row r="144" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D144" s="1"/>
+      <c r="E144" s="1"/>
+    </row>
+    <row r="145" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D145" s="1"/>
+      <c r="E145" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Some mouse macros + changing startup script
</commit_message>
<xml_diff>
--- a/scripts f keys taken.xlsx
+++ b/scripts f keys taken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\ahk\ahk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EF9CA3-BFFB-4ACC-AC19-3927285D48C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C79A34-4BB8-4C86-9106-D18A5394FECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2700" windowWidth="29040" windowHeight="15840" xr2:uid="{988935E9-0B57-47DD-B8E6-A709369EFA7D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="106">
   <si>
     <t>f1</t>
   </si>
@@ -120,9 +120,6 @@
     <t>streamdeck</t>
   </si>
   <si>
-    <t>mouse</t>
-  </si>
-  <si>
     <t>putting things here requires being careful</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
   </si>
   <si>
     <t>audio gain</t>
-  </si>
-  <si>
-    <t>highlight search box</t>
   </si>
   <si>
     <t>scale effects</t>
@@ -259,9 +253,6 @@
     <t>ctrl+alt+shift+w -&gt; warp to main monitor</t>
   </si>
   <si>
-    <t>ctrl + middle mouse click</t>
-  </si>
-  <si>
     <t>NumLock</t>
   </si>
   <si>
@@ -289,18 +280,12 @@
     <t>Second Keyboard</t>
   </si>
   <si>
-    <t>backspace</t>
-  </si>
-  <si>
     <t>all mii wii song</t>
   </si>
   <si>
     <t>.</t>
   </si>
   <si>
-    <t>enter</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
@@ -350,6 +335,24 @@
   </si>
   <si>
     <t>input manual scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + scrolling = accelerated scrolling</t>
+  </si>
+  <si>
+    <t>NumLock + 1</t>
+  </si>
+  <si>
+    <t>input manual gain</t>
+  </si>
+  <si>
+    <t>mouse button (nudge track)</t>
+  </si>
+  <si>
+    <t>mouse button (insert goose sfx)</t>
+  </si>
+  <si>
+    <t>mouse button (not assigned yet)</t>
   </si>
 </sst>
 </file>
@@ -415,12 +418,74 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -430,7 +495,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -446,6 +511,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -763,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6D84AE-EF5D-416A-8D76-EC512DB5CC0A}">
-  <dimension ref="A2:J145"/>
+  <dimension ref="A2:J146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,7 +860,7 @@
   <sheetData>
     <row r="2" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
@@ -797,13 +873,13 @@
         <v>26</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
@@ -848,7 +924,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1"/>
       <c r="H7" s="1"/>
@@ -861,7 +937,7 @@
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
@@ -870,7 +946,7 @@
         <v>6</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="3"/>
+      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
@@ -900,10 +976,10 @@
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="1"/>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
@@ -924,7 +1000,7 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="3"/>
+      <c r="G14" s="1"/>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
@@ -934,7 +1010,6 @@
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="3"/>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
@@ -942,146 +1017,157 @@
       <c r="D16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E16" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="10"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E17" s="13"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="16"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="3"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="3"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="3"/>
       <c r="H20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E21" s="9"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E22" s="13"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="16"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="3"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F24" s="1"/>
-      <c r="G24" s="3"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="3"/>
+      <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="3"/>
+      <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D30" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D31" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D32" s="1" t="s">
         <v>3</v>
       </c>
@@ -1096,6 +1182,7 @@
       <c r="D34" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G34" s="3"/>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D35" s="1" t="s">
@@ -1116,6 +1203,7 @@
       <c r="D38" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="G38" s="3"/>
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D39" s="1" t="s">
@@ -1131,6 +1219,7 @@
       <c r="D41" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G41" s="3"/>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D42" s="1" t="s">
@@ -1146,49 +1235,54 @@
       <c r="D44" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="G44" s="3"/>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D45" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="G45" s="3"/>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D46" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="G46" s="3"/>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D47" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="G47" s="3"/>
       <c r="I47" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D48" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G48" s="3"/>
       <c r="I48" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D49" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G49" s="1"/>
+      <c r="G49" s="3"/>
       <c r="I49" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D50" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G50" s="1"/>
+      <c r="G50" s="3"/>
       <c r="I50" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
@@ -1197,7 +1291,7 @@
       </c>
       <c r="G51" s="3"/>
       <c r="I51" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
@@ -1208,7 +1302,7 @@
     </row>
     <row r="55" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C55" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D55" s="6">
         <v>1</v>
@@ -1225,6 +1319,7 @@
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
@@ -1235,6 +1330,7 @@
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
@@ -1245,9 +1341,7 @@
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
-      <c r="G58" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
@@ -1297,84 +1391,84 @@
     </row>
     <row r="64" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="65" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="67" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D70" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="73" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="75" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>27</v>
@@ -1382,110 +1476,105 @@
     </row>
     <row r="78" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D78" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J78" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="79" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D79" s="1"/>
       <c r="E79" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="80" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D80" s="1"/>
       <c r="E80" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D81" s="1"/>
       <c r="E81" s="8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D82" s="1"/>
       <c r="E82" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H82" s="1"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D83" s="1"/>
       <c r="E83" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H83" s="1"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E84" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E85" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G85" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G86" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D90" s="6">
         <v>0</v>
@@ -1504,7 +1593,7 @@
         <v>2</v>
       </c>
       <c r="G92" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -1520,7 +1609,7 @@
         <v>4</v>
       </c>
       <c r="G94" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -1529,7 +1618,7 @@
         <v>5</v>
       </c>
       <c r="G95" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -1538,7 +1627,7 @@
         <v>6</v>
       </c>
       <c r="G96" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="97" spans="3:10" x14ac:dyDescent="0.25">
@@ -1547,10 +1636,10 @@
         <v>7</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J97" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="98" spans="3:10" x14ac:dyDescent="0.25">
@@ -1559,10 +1648,10 @@
         <v>8</v>
       </c>
       <c r="G98" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J98" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="99" spans="3:10" x14ac:dyDescent="0.25">
@@ -1571,87 +1660,88 @@
         <v>9</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J99" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="100" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="101" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C101" s="1"/>
       <c r="D101" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="102" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="103" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D103" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F103"/>
     </row>
     <row r="104" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D104" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G104" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="105" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="106" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D106" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G106" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="107" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C108" s="1"/>
-      <c r="D108" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F108" s="1"/>
-    </row>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="107" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D107" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G107" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="108" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="109" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C109" s="1"/>
-      <c r="D109" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="D109" s="1"/>
+      <c r="F109" s="1"/>
     </row>
     <row r="110" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C110" s="1"/>
       <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
     </row>
     <row r="111" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
     </row>
     <row r="112" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D112" s="1"/>
@@ -1682,7 +1772,6 @@
     </row>
     <row r="121" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D121" s="1"/>
-      <c r="E121" s="1"/>
     </row>
     <row r="122" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D122" s="1"/>
@@ -1779,6 +1868,10 @@
     <row r="145" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
+    </row>
+    <row r="146" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D146" s="1"/>
+      <c r="E146" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
small corrections to move project
</commit_message>
<xml_diff>
--- a/scripts f keys taken.xlsx
+++ b/scripts f keys taken.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\ahk\ahk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C79A34-4BB8-4C86-9106-D18A5394FECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB41EBAE-1179-4E1C-88A5-E39AD614173C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2700" windowWidth="29040" windowHeight="15840" xr2:uid="{988935E9-0B57-47DD-B8E6-A709369EFA7D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{988935E9-0B57-47DD-B8E6-A709369EFA7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="108">
   <si>
     <t>f1</t>
   </si>
@@ -241,9 +241,6 @@
     <t>ctrl+shift+c -&gt; google searches highlighted text</t>
   </si>
   <si>
-    <t>caps+z -&gt; add audio keyframe</t>
-  </si>
-  <si>
     <t>alt+c -&gt; crop preset</t>
   </si>
   <si>
@@ -353,6 +350,15 @@
   </si>
   <si>
     <t>mouse button (not assigned yet)</t>
+  </si>
+  <si>
+    <t>mouse button (insert bleep sfx)</t>
+  </si>
+  <si>
+    <t>caps+z -&gt; zoom out</t>
+  </si>
+  <si>
+    <t>mouse buttons</t>
   </si>
 </sst>
 </file>
@@ -495,7 +501,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -513,7 +519,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -842,7 +847,7 @@
   <dimension ref="A2:J146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,7 +884,7 @@
         <v>32</v>
       </c>
       <c r="J2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
@@ -1013,36 +1018,38 @@
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>100</v>
+      <c r="E16" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="F16" s="10"/>
-      <c r="G16" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="H16" s="18" t="s">
+      <c r="G16" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="H16" s="17" t="s">
         <v>30</v>
       </c>
       <c r="I16" s="10"/>
-      <c r="J16" s="12"/>
+      <c r="J16" s="11"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="19" t="s">
+      <c r="E17" s="12"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="16"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="15"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
@@ -1050,7 +1057,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F18" s="1"/>
       <c r="H18" s="1"/>
@@ -1079,32 +1086,34 @@
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="D21" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="11" t="s">
-        <v>105</v>
+      <c r="G21" s="17" t="s">
+        <v>103</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="12"/>
+      <c r="J21" s="11"/>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="15" t="s">
+      <c r="E22" s="12"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="16"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="15"/>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
@@ -1273,7 +1282,7 @@
       </c>
       <c r="G49" s="3"/>
       <c r="I49" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
@@ -1412,15 +1421,15 @@
     </row>
     <row r="67" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
+        <v>72</v>
+      </c>
+      <c r="D70" t="s">
         <v>73</v>
-      </c>
-      <c r="D70" t="s">
-        <v>74</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>63</v>
@@ -1428,47 +1437,47 @@
     </row>
     <row r="71" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="75" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="76" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>27</v>
@@ -1483,13 +1492,13 @@
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J78" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="79" spans="3:10" x14ac:dyDescent="0.25">
@@ -1499,7 +1508,7 @@
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>39</v>
@@ -1521,7 +1530,7 @@
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D81" s="1"/>
       <c r="E81" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="8" t="s">
@@ -1538,7 +1547,7 @@
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H82" s="1"/>
     </row>
@@ -1549,16 +1558,16 @@
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="8" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="H83" s="1"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E84" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -1566,12 +1575,12 @@
         <v>67</v>
       </c>
       <c r="G85" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>44</v>
@@ -1678,7 +1687,7 @@
     <row r="101" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C101" s="1"/>
       <c r="D101" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="102" spans="3:10" x14ac:dyDescent="0.25">
@@ -1687,7 +1696,7 @@
         <v>61</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="103" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1695,13 +1704,13 @@
         <v>62</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F103"/>
     </row>
     <row r="104" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D104" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G104" s="8" t="s">
         <v>54</v>
@@ -1710,23 +1719,23 @@
     <row r="105" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="106" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D106" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G106" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="G106" s="8" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="107" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D107" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G107" s="8" t="s">
         <v>101</v>
-      </c>
-      <c r="G107" s="8" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="108" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>